<commit_message>
More read test, more test files and improved read_xls function
</commit_message>
<xml_diff>
--- a/tests/sample.xlsx
+++ b/tests/sample.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\workspace\python projects\learn\xls_tools\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FD8829-369C-4F22-8333-906D3AD872D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDFE51E-ACEC-4B2A-97F5-5EAA9D44ED24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="productos" sheetId="1" r:id="rId1"/>
-    <sheet name="reducido" sheetId="3" r:id="rId2"/>
+    <sheet name="Products" sheetId="1" r:id="rId1"/>
+    <sheet name="Resume" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="118">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>Title</t>
   </si>
@@ -60,9 +57,6 @@
     <t>Operator</t>
   </si>
   <si>
-    <t>81f809e4-1179-4991-b2ab-7105694ad355</t>
-  </si>
-  <si>
     <t>Guided tour of the Alhambra and Generalife in Premium tour</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>Granada</t>
   </si>
   <si>
-    <t>da41cbcb-b0cc-4ae1-9db9-b32fdfd6de99</t>
-  </si>
-  <si>
     <t>Guided tour of the Alhambra and Generalife in Small group</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
     <t>02 TOUR ALHAMBRA 20</t>
   </si>
   <si>
-    <t>6fa6919e-1b90-4152-9f41-db4858d6361f</t>
-  </si>
-  <si>
     <t>Guided tour of the Alhambra and Generalife in Regular group</t>
   </si>
   <si>
@@ -99,9 +87,6 @@
     <t>03 TOUR ALHAMBRA 30</t>
   </si>
   <si>
-    <t>3807c6e4-662f-4160-a0ce-529f2a37b7bf</t>
-  </si>
-  <si>
     <t>Guided tour of the Alhambra gardens, Alcazaba and Generalife in Regular group</t>
   </si>
   <si>
@@ -111,9 +96,6 @@
     <t>04 TOUR JARDINES 30</t>
   </si>
   <si>
-    <t>5bd0dcdd-6990-464d-b040-84f9b091d7ab</t>
-  </si>
-  <si>
     <t>COMBO: GUIDED TOUR TO ALHAMBRA + ALBAICIN &amp; SACROMONTE</t>
   </si>
   <si>
@@ -123,9 +105,6 @@
     <t>05 TOUR ALHAMBRA+ALBAICIN 30</t>
   </si>
   <si>
-    <t>aef322b1-695d-471f-bbc7-29d7aa924cd7</t>
-  </si>
-  <si>
     <t>Combo: Guided Tour to Cathedral and Roya Chapel + Alhambra  and Generalife</t>
   </si>
   <si>
@@ -135,9 +114,6 @@
     <t>06 TOUR CATEDRAL+ALHAMBRA 30</t>
   </si>
   <si>
-    <t>8f14a966-24b2-41b8-b3d4-4ef80d9b1fdd</t>
-  </si>
-  <si>
     <t>Guided visit to the Cathedral and Royal Chapel</t>
   </si>
   <si>
@@ -147,9 +123,6 @@
     <t>11 TOUR CATEDRAL/CAPILLA 30</t>
   </si>
   <si>
-    <t>ff48f009-5819-4bb3-b164-9ad082041488</t>
-  </si>
-  <si>
     <t>Albaicin and Sacromonte guided tour</t>
   </si>
   <si>
@@ -159,9 +132,6 @@
     <t>12 TOUR ALBAICIN  30</t>
   </si>
   <si>
-    <t>e87edede-3819-4d22-b712-8695203c40b5</t>
-  </si>
-  <si>
     <t>Guided visit to the Cathedral and Royal Chapel + Albaicin and Sacromonte</t>
   </si>
   <si>
@@ -171,9 +141,6 @@
     <t>13 TOUR CATEDRAL+ ALBAICIN 30</t>
   </si>
   <si>
-    <t>98131131-e9de-4055-ae0b-5fcc0d5e9448</t>
-  </si>
-  <si>
     <t>Private guided tour of the Alhambra and Generalife</t>
   </si>
   <si>
@@ -183,9 +150,6 @@
     <t>15 PRIVATE TOUR GRX</t>
   </si>
   <si>
-    <t>5336cd41-baae-4aac-b6fe-30b0b6fec5eb</t>
-  </si>
-  <si>
     <t>Albaicin and Sacromonte Private Tour</t>
   </si>
   <si>
@@ -195,9 +159,6 @@
     <t>16 PRIVATE TOUR GRX</t>
   </si>
   <si>
-    <t>777a2632-ec84-4b31-9ba9-9c61c57dfc21</t>
-  </si>
-  <si>
     <t>Alhambra and Generalife Private Tour</t>
   </si>
   <si>
@@ -207,9 +168,6 @@
     <t>17 PRIVATE TOUR GRX</t>
   </si>
   <si>
-    <t>795bd38b-caa5-4b38-aa91-73b7d86c7376</t>
-  </si>
-  <si>
     <t>Cathedral and Royal Chapel of Granada. Private Tour</t>
   </si>
   <si>
@@ -219,9 +177,6 @@
     <t>18 PRIVATE TOUR GRX</t>
   </si>
   <si>
-    <t>6dab8be1-6a0d-4434-9fb1-09b63190777e</t>
-  </si>
-  <si>
     <t>Cathedral and Royal Chapel + Albaicín and Sacromonte Private Tour</t>
   </si>
   <si>
@@ -231,9 +186,6 @@
     <t>19 PRIVATE TOUR GRX</t>
   </si>
   <si>
-    <t>d8b2c951-e880-4688-9f50-723385a97950</t>
-  </si>
-  <si>
     <t>Sagrada Familia: Skip the line guided tour with official guide</t>
   </si>
   <si>
@@ -246,9 +198,6 @@
     <t>Barcelona</t>
   </si>
   <si>
-    <t>1737de0b-b8e9-4e8d-8f92-17dbba9683ee</t>
-  </si>
-  <si>
     <t>Sagrada Familia: Skip the line guided tour with official guide Premium Group</t>
   </si>
   <si>
@@ -258,9 +207,6 @@
     <t>21 TOUR SAFA 10</t>
   </si>
   <si>
-    <t>4865efe2-da85-41dd-bf72-21d6bc15bd65</t>
-  </si>
-  <si>
     <t>Guided tour of Park Guell</t>
   </si>
   <si>
@@ -270,9 +216,6 @@
     <t>22 TOUR PG 30</t>
   </si>
   <si>
-    <t>260ba2a0-d828-42f1-8bd5-7d7c6c300942</t>
-  </si>
-  <si>
     <t>Combo: Guided tour to Sagrada Familia and Park Güell</t>
   </si>
   <si>
@@ -282,9 +225,6 @@
     <t>23 TOUR SAFA-PARK 30</t>
   </si>
   <si>
-    <t>1b6d0fcb-c040-4bcb-ba12-7a6a311e2fd1</t>
-  </si>
-  <si>
     <t>Guided Tour to Seville Cathedral</t>
   </si>
   <si>
@@ -297,9 +237,6 @@
     <t>Sevilla</t>
   </si>
   <si>
-    <t>ab7194ac-1062-4227-8cf8-84cde221cf5b</t>
-  </si>
-  <si>
     <t>GUIDED TOUR TO THE ALCAZAR OF SEVILLE IN ENGLISH</t>
   </si>
   <si>
@@ -309,9 +246,6 @@
     <t>31 TOUR TO THE ALCAZAR 30</t>
   </si>
   <si>
-    <t>84faa6b7-1e24-4767-9906-c09d27e6d12a</t>
-  </si>
-  <si>
     <t>GUIDED TOUR TO THE ALCAZAR + SEVILLE CATHEDRAL IN ENGLISH</t>
   </si>
   <si>
@@ -321,9 +255,6 @@
     <t>32 TOUR TO THE ALCAZAR + SEVILLE CATHEDRAL 30</t>
   </si>
   <si>
-    <t>8fa1b629-94f2-41c9-a853-86b39f89d026</t>
-  </si>
-  <si>
     <t>Guided tour Royal Palace of Madrid</t>
   </si>
   <si>
@@ -336,9 +267,6 @@
     <t>Madrid</t>
   </si>
   <si>
-    <t>05e286a7-feca-4261-ad37-65ebb5de5213</t>
-  </si>
-  <si>
     <t>Guided tour Royal Palace of Madrid Premium Group</t>
   </si>
   <si>
@@ -348,9 +276,6 @@
     <t>41 TOUR PALACIO REAL 8</t>
   </si>
   <si>
-    <t>ed755795-3581-4ca3-a3c2-a076dc25bdcb</t>
-  </si>
-  <si>
     <t>Visita Guiada a la Mezquita Catedral de Cordoba</t>
   </si>
   <si>
@@ -363,9 +288,6 @@
     <t>Cordoba</t>
   </si>
   <si>
-    <t>672cc685-bffe-44b3-b26c-ef7e92040fd7</t>
-  </si>
-  <si>
     <t>Guided tour of the Caminito del Rey</t>
   </si>
   <si>
@@ -382,12 +304,6 @@
   </si>
   <si>
     <t>Rezdy ID</t>
-  </si>
-  <si>
-    <t>Revisar filas en rojo para ventas visita pasada</t>
-  </si>
-  <si>
-    <t>Filas en rojo sin ventas visitas futuro</t>
   </si>
 </sst>
 </file>
@@ -778,21 +694,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.796875" customWidth="1"/>
-    <col min="2" max="2" width="69.09765625" customWidth="1"/>
-    <col min="3" max="3" width="31.69921875" customWidth="1"/>
-    <col min="6" max="6" width="41" customWidth="1"/>
+    <col min="1" max="1" width="69.09765625" customWidth="1"/>
+    <col min="2" max="2" width="31.69921875" customWidth="1"/>
+    <col min="5" max="5" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -815,598 +730,510 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
         <v>28</v>
       </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
         <v>40</v>
       </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>43</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B14" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>47</v>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="B15" t="s">
         <v>48</v>
       </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>50</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B16" t="s">
         <v>51</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
         <v>52</v>
       </c>
-      <c r="G12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="F16" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B17" t="s">
         <v>55</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
         <v>56</v>
       </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="F17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B18" t="s">
         <v>58</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
         <v>59</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="F18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F19" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>63</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="B20" t="s">
         <v>64</v>
       </c>
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
         <v>65</v>
       </c>
-      <c r="B16" t="s">
+      <c r="F20" t="s">
         <v>66</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>67</v>
       </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="B21" t="s">
         <v>68</v>
       </c>
-      <c r="G16" t="s">
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>70</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B22" t="s">
         <v>71</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>72</v>
       </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>73</v>
       </c>
-      <c r="G17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B23" t="s">
         <v>74</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
         <v>75</v>
       </c>
-      <c r="C18" t="s">
+      <c r="F23" t="s">
         <v>76</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>77</v>
       </c>
-      <c r="G18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="B24" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="C25" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B20" t="s">
+      <c r="F25" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="B26" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G20" t="s">
+      <c r="C26" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="F26" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B21" t="s">
+      <c r="H26" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B22" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>98</v>
-      </c>
-      <c r="G23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>103</v>
-      </c>
-      <c r="G24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F556A9BB-2D55-4F12-B3EF-0F1E4580F52A}">
   <dimension ref="B1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1431,202 +1258,202 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>